<commit_message>
final clean version of data and cheat sheet
</commit_message>
<xml_diff>
--- a/Data/cheat sheet .xlsx
+++ b/Data/cheat sheet .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmybelloni/cs257labs/cs257-s21-team-f/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF539EA1-A602-4849-A35D-4197867C95CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF90134C-3C0C-D444-B736-937D931CCB11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{EA59D4E6-F119-224E-A9C4-FCC973200CC9}"/>
+    <workbookView xWindow="5440" yWindow="460" windowWidth="21120" windowHeight="16120" xr2:uid="{EA59D4E6-F119-224E-A9C4-FCC973200CC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="164">
   <si>
     <t xml:space="preserve">Taken all together, how would you say things are in your life these days--would you say that you are (very happy), somewhat happy, or (not too happy)? </t>
   </si>
@@ -61,9 +61,6 @@
     <t>Are you a member of a social group</t>
   </si>
   <si>
-    <t>Are you a member of a service organization</t>
-  </si>
-  <si>
     <t>How often do you participate in meetings with this group?</t>
   </si>
   <si>
@@ -278,6 +275,258 @@
   </si>
   <si>
     <t>How big a problem would you say being lonely is for you?</t>
+  </si>
+  <si>
+    <t>Happiness</t>
+  </si>
+  <si>
+    <t>Finances</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Companionship</t>
+  </si>
+  <si>
+    <t>Isolated</t>
+  </si>
+  <si>
+    <t>Lonely</t>
+  </si>
+  <si>
+    <t>Neighbors</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t>Nonprofits</t>
+  </si>
+  <si>
+    <t>Churches</t>
+  </si>
+  <si>
+    <t>Factors</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Unemployment</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Counselor</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>Drugs</t>
+  </si>
+  <si>
+    <t>Cigarettes</t>
+  </si>
+  <si>
+    <t>Overeat</t>
+  </si>
+  <si>
+    <t>Past</t>
+  </si>
+  <si>
+    <t>Browse</t>
+  </si>
+  <si>
+    <t>Distract</t>
+  </si>
+  <si>
+    <t>Talk</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Helpful</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Afford</t>
+  </si>
+  <si>
+    <t>FamilyLife</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>SocialGroup</t>
+  </si>
+  <si>
+    <t>SocialGroupFrequency</t>
+  </si>
+  <si>
+    <t>ServiceOrganization</t>
+  </si>
+  <si>
+    <t>SOrganizationFrequency</t>
+  </si>
+  <si>
+    <t>HWFrequency</t>
+  </si>
+  <si>
+    <t>HealthWellness</t>
+  </si>
+  <si>
+    <t>LonelinessFrequency</t>
+  </si>
+  <si>
+    <t>LeftOut</t>
+  </si>
+  <si>
+    <t>Discuss</t>
+  </si>
+  <si>
+    <t>FamilyInPerson</t>
+  </si>
+  <si>
+    <t>FamilyOverPhone</t>
+  </si>
+  <si>
+    <t>FamilyOverSocialMedia</t>
+  </si>
+  <si>
+    <t>FriendsInPerson</t>
+  </si>
+  <si>
+    <t>FriendsOverPhone</t>
+  </si>
+  <si>
+    <t>FriendsOverSocialMedia</t>
+  </si>
+  <si>
+    <t>PublicOrIndividual</t>
+  </si>
+  <si>
+    <t>MovingAway</t>
+  </si>
+  <si>
+    <t>GovernmentCuts</t>
+  </si>
+  <si>
+    <t>AgingParents</t>
+  </si>
+  <si>
+    <t>SocialMedia</t>
+  </si>
+  <si>
+    <t>SocialMediaFrequency</t>
+  </si>
+  <si>
+    <t>SocialMediaHours</t>
+  </si>
+  <si>
+    <t>LookingOrEngaging</t>
+  </si>
+  <si>
+    <t>LonelinessAndSocialMedia</t>
+  </si>
+  <si>
+    <t>OnlineVsPhone</t>
+  </si>
+  <si>
+    <t>OnlineVsInPerson</t>
+  </si>
+  <si>
+    <t>RecommendInternet</t>
+  </si>
+  <si>
+    <t>SpendTime</t>
+  </si>
+  <si>
+    <t>BigProblem</t>
+  </si>
+  <si>
+    <t>LengthLonely</t>
+  </si>
+  <si>
+    <t>ImpactPersonalRelationships</t>
+  </si>
+  <si>
+    <t>ImpactJob</t>
+  </si>
+  <si>
+    <t>ImpactPhysicalHealth</t>
+  </si>
+  <si>
+    <t>ImpactMentalHealth</t>
+  </si>
+  <si>
+    <t>TalkFriend</t>
+  </si>
+  <si>
+    <t>VisitPublic</t>
+  </si>
+  <si>
+    <t>CloseFriend</t>
+  </si>
+  <si>
+    <t>FamilyMember</t>
+  </si>
+  <si>
+    <t>MentalHealthProfessional</t>
+  </si>
+  <si>
+    <t>Advisor</t>
+  </si>
+  <si>
+    <t>WhoToTalkTo</t>
+  </si>
+  <si>
+    <t>ProblemNotBad</t>
+  </si>
+  <si>
+    <t>HandleOnYourOwn</t>
+  </si>
+  <si>
+    <t>ViolentAct</t>
+  </si>
+  <si>
+    <t>HarmingYourself</t>
+  </si>
+  <si>
+    <t>Sometimes loneliness is caused by a specific event or condition such as the loss of a spouse or an unexpected illness, and sometimes there doesn’t seem to be a specific reason why people feel lonely. Would you say there is a specific cause for your feelin</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>Cause</t>
+  </si>
+  <si>
+    <t>HaveTime</t>
   </si>
 </sst>
 </file>
@@ -640,430 +889,680 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864BBDF0-EB5B-2D45-84FD-1E286A8A2E1C}">
-  <dimension ref="A1:A83"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="155" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="155" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>152</v>
+      </c>
+      <c r="B72" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>110</v>
+      </c>
+      <c r="B75" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>156</v>
+      </c>
+      <c r="B77" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>163</v>
+      </c>
+      <c r="B78" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>111</v>
+      </c>
+      <c r="B79" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed buttons, made basic dropdown menus
</commit_message>
<xml_diff>
--- a/Data/cheat sheet .xlsx
+++ b/Data/cheat sheet .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmybelloni/cs257labs/cs257-s21-team-f/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF90134C-3C0C-D444-B736-937D931CCB11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE31B3A3-6915-2B49-8DB8-967F34A91918}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5440" yWindow="460" windowWidth="21120" windowHeight="16120" xr2:uid="{EA59D4E6-F119-224E-A9C4-FCC973200CC9}"/>
   </bookViews>
@@ -517,9 +517,6 @@
     <t>HarmingYourself</t>
   </si>
   <si>
-    <t>Sometimes loneliness is caused by a specific event or condition such as the loss of a spouse or an unexpected illness, and sometimes there doesn’t seem to be a specific reason why people feel lonely. Would you say there is a specific cause for your feelin</t>
-  </si>
-  <si>
     <t>Connections</t>
   </si>
   <si>
@@ -527,6 +524,9 @@
   </si>
   <si>
     <t>HaveTime</t>
+  </si>
+  <si>
+    <t>Are you a member of a service organization?</t>
   </si>
 </sst>
 </file>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864BBDF0-EB5B-2D45-84FD-1E286A8A2E1C}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,7 +986,7 @@
         <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1255,7 +1255,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B45" t="s">
         <v>41</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>47</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B78" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
two variable scatter added
</commit_message>
<xml_diff>
--- a/Data/cheat sheet .xlsx
+++ b/Data/cheat sheet .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmybelloni/cs257labs/cs257-s21-team-f/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3312521-2CAC-9145-840A-7F7A12E99E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B278F1F7-80E8-F44B-9812-27607BBA4F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5440" yWindow="460" windowWidth="21120" windowHeight="16120" xr2:uid="{EA59D4E6-F119-224E-A9C4-FCC973200CC9}"/>
   </bookViews>
@@ -36,18 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="164">
   <si>
-    <t>Please tell us whether you are satisfied or dissatisfied with your family life</t>
-  </si>
-  <si>
-    <t>Please tell us whether you are satisfied or dissatisfied with your personal financial situation</t>
-  </si>
-  <si>
-    <t>Please tell us whether you are satisfied or dissatisfied with your current employment situation</t>
-  </si>
-  <si>
-    <t>Please tell us whether you are satisfied or dissatisfied with your current housing situation</t>
-  </si>
-  <si>
     <t>Thinking about your personal support network – that is relatives and friends living nearby who
 you can rely on for help or support – do you have a lot of people you can rely on, a fair amount, just a few, or no people living nearby who you can rely on?</t>
   </si>
@@ -527,6 +515,18 @@
   </si>
   <si>
     <t>Taken all together, how would you say things are in your life these days?</t>
+  </si>
+  <si>
+    <t>Please tell us whether you are satisfied or dissatisfied with your family life?</t>
+  </si>
+  <si>
+    <t>Please tell us whether you are satisfied or dissatisfied with your personal financial situation?</t>
+  </si>
+  <si>
+    <t>Please tell us whether you are satisfied or dissatisfied with your current employment situation?</t>
+  </si>
+  <si>
+    <t>Please tell us whether you are satisfied or dissatisfied with your current housing situation?</t>
   </si>
 </sst>
 </file>
@@ -549,12 +549,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -569,12 +587,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864BBDF0-EB5B-2D45-84FD-1E286A8A2E1C}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,666 +924,666 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>130</v>
-      </c>
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>131</v>
-      </c>
-      <c r="B36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B53" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B60" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>132</v>
-      </c>
-      <c r="B38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>133</v>
-      </c>
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>134</v>
-      </c>
-      <c r="B42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>135</v>
-      </c>
-      <c r="B43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>136</v>
-      </c>
-      <c r="B44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>159</v>
-      </c>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>137</v>
-      </c>
-      <c r="B46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>139</v>
-      </c>
-      <c r="B48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>140</v>
-      </c>
-      <c r="B49" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>141</v>
-      </c>
-      <c r="B50" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>142</v>
-      </c>
-      <c r="B51" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>160</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="B63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B53" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>143</v>
-      </c>
-      <c r="B54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>144</v>
-      </c>
-      <c r="B55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B56" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B64" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B68" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B69" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B70" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B57" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B58" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B72" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B59" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B60" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>99</v>
-      </c>
-      <c r="B61" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>100</v>
-      </c>
-      <c r="B62" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>101</v>
-      </c>
-      <c r="B63" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>102</v>
-      </c>
-      <c r="B64" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>103</v>
-      </c>
-      <c r="B65" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>104</v>
-      </c>
-      <c r="B66" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B74" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B67" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="B75" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B68" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B79" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B69" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>108</v>
-      </c>
-      <c r="B70" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>150</v>
-      </c>
-      <c r="B71" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>151</v>
-      </c>
-      <c r="B72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>152</v>
-      </c>
-      <c r="B73" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="B81" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B74" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>109</v>
-      </c>
-      <c r="B75" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="B82" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B76" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>155</v>
-      </c>
-      <c r="B77" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>161</v>
-      </c>
-      <c r="B78" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>110</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="B83" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>156</v>
-      </c>
-      <c r="B80" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>111</v>
-      </c>
-      <c r="B81" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>157</v>
-      </c>
-      <c r="B82" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>158</v>
-      </c>
-      <c r="B83" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>